<commit_message>
bank application with checks and junit
</commit_message>
<xml_diff>
--- a/transactionInBank/checklist.xlsx
+++ b/transactionInBank/checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\trainee\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\trainee\Desktop\PoojaShare\16april\transactionInBank\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
   <si>
     <t>1.pmd</t>
   </si>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +601,15 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>